<commit_message>
11-12-15 2:39 PM Lynn
Changes to gitignore because changed Small SNPs data.
</commit_message>
<xml_diff>
--- a/data/Small SNPs.xlsx
+++ b/data/Small SNPs.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="All Samples, 5 SNPs" sheetId="1" r:id="rId1"/>
+    <sheet name="49 Samples, 5 SNPs" sheetId="2" r:id="rId2"/>
+    <sheet name="Random #2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t>rs3094315</t>
   </si>
@@ -374,8 +374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F681"/>
   <sheetViews>
-    <sheetView topLeftCell="A674" workbookViewId="0">
-      <selection activeCell="F682" sqref="F682"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection sqref="A1:F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14009,8 +14009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15025,12 +15025,1015 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>0</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>0</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>0</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>